<commit_message>
set case id to 0 to avoid to be run with suite all.cs
</commit_message>
<xml_diff>
--- a/xdoc/test-case.xlsx
+++ b/xdoc/test-case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/dev/go/zentaoatf/xdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{905DCFB7-B875-204C-960C-67532B2663FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BABFEA7-606E-8C45-9D82-F7AC1981CAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33280" windowHeight="20540" xr2:uid="{02BAE9CC-3948-864F-A7A3-2466404408E9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="94">
   <si>
     <t>Up</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,10 +119,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>更新用例标题到禅道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>提交测试结果到禅道</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -217,131 +213,170 @@
     <t>ztf.exe help</t>
   </si>
   <si>
+    <t>ztf.exe co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe ci scripts\tc-1.php </t>
+  </si>
+  <si>
+    <t>ztf.exe update -p 1 -m 15 -l php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe .\ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run . </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe scripts\all.cs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run scripts scripts\all.cs </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe scripts\all.cs scripts </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run logs\2019-09-04\result.txt </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe logs\2019-09-04\result.json </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -s 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run scripts -s 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -t 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run scripts -t 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe cr logs\2019-09-04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe cb logs\2019-09-04 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe list scripts\用例模块A scripts\tc-1.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe ls scripts\用例模块A\ scripts\tc-1.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 新闻  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe view scripts\用例模块A scripts\tc-1.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v scripts\用例模块A scripts\tc-1.php -k 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v scripts\用例模块A\ scripts\tc-1.php -k 新闻  </t>
+  </si>
+  <si>
+    <t>ztf.exe win_line_break.bat</t>
+  </si>
+  <si>
+    <t>ztf.exe demo\sample</t>
+  </si>
+  <si>
+    <t>ztf demo\sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf demo\lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atf.exe sort demo\sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">atf.exe clean </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重排脚本中的步骤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除执行日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ztf.exe -h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ztf.exe set</t>
-  </si>
-  <si>
-    <t>ztf.exe co</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ztf.exe co -m 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>ztf.exe co -p 1 -m 15 -l php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe ci scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t>ztf.exe update -p 1 -m 15 -l php</t>
-  </si>
-  <si>
-    <t>ztf.exe up -p 1 -m 15 -l php</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe .\ </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe scripts </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe \Users\aaron\dev\go\zentaoatf\scripts-demo\tc-01.sh </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe c:\Users\admin\atf\scripts </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe scripts\all.cs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run scripts scripts\all.cs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe scripts\all.cs scripts </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run logs\2019-09-04\result.txt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe logs\2019-09-04\result.json </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -s 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run scripts -s 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -t 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run scripts -t 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe cr logs\2019-09-04 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe cb logs\2019-09-04 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe list scripts\用例模块A scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe ls scripts\用例模块A\ scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 新闻  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe view scripts\用例模块A scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v scripts\用例模块A scripts\tc-1.php -k 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v scripts\用例模块A\ scripts\tc-1.php -k 新闻  </t>
-  </si>
-  <si>
-    <t>ztf.exe win_line_break.bat</t>
-  </si>
-  <si>
-    <t>ztf.exe demo\sample</t>
-  </si>
-  <si>
-    <t>ztf demo\sample</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf demo\lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新用例到禅道(TODO)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe up -p 1 -l php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe demo\lang\php </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\2_webpage_extract.php</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -386,6 +421,19 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -401,7 +449,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -461,13 +509,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -499,6 +573,27 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -815,22 +910,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6013D07F-3FC9-2B42-A079-965085852FDE}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="58.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="39.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" customHeight="1">
+    <row r="1" spans="1:6" ht="20" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -838,607 +934,727 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1">
+    <row r="2" spans="1:6" ht="20" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1">
+      <c r="E2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A3" s="9"/>
-      <c r="B3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="20" customHeight="1">
+      <c r="E3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20" customHeight="1">
       <c r="A4" s="9"/>
       <c r="B4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>30</v>
+        <v>84</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="20" customHeight="1">
+        <v>29</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
       <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1">
+      <c r="E5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>31</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="20" customHeight="1">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="20" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="E7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="15" customFormat="1" ht="20" customHeight="1">
+      <c r="A8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="20" customHeight="1">
+      <c r="B8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="20" customHeight="1">
+      <c r="E9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="20" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C10" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="20" customHeight="1">
+      <c r="E10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="20" customHeight="1">
       <c r="A11" s="9" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="20" customHeight="1">
+      <c r="E11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="20" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="20" customHeight="1">
+      <c r="E12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="20" customHeight="1">
       <c r="A13" s="9"/>
       <c r="B13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="20" customHeight="1">
+      <c r="E13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="20" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="20" customHeight="1">
+      <c r="E14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20" customHeight="1">
       <c r="A15" s="9"/>
       <c r="B15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="20" customHeight="1">
+      <c r="E15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="20" customHeight="1">
       <c r="A16" s="9"/>
       <c r="B16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="20" customHeight="1">
+      <c r="E16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="20" customHeight="1">
       <c r="A17" s="9"/>
       <c r="B17" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
+        <v>92</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="20" customHeight="1">
+        <v>31</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="20" customHeight="1">
       <c r="A18" s="9"/>
       <c r="B18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="C18" s="5"/>
       <c r="D18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="1:5" ht="20" customHeight="1">
+        <v>32</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="20" customHeight="1">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="20" customHeight="1">
+      <c r="E19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="20" customHeight="1">
       <c r="A20" s="9"/>
       <c r="B20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="1:5" ht="20" customHeight="1">
+      <c r="E20" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" ht="20" customHeight="1">
       <c r="A21" s="9"/>
       <c r="B21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>34</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="1:5" ht="20" customHeight="1">
+        <v>33</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="20" customHeight="1">
       <c r="A22" s="9"/>
       <c r="B22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="1:5" ht="20" customHeight="1">
+      <c r="E22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="20" customHeight="1">
       <c r="A23" s="9"/>
       <c r="B23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="1:5" ht="20" customHeight="1">
+      <c r="E23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="20" customHeight="1">
       <c r="A24" s="9"/>
       <c r="B24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="1:5" ht="20" customHeight="1">
+      <c r="E24" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="20" customHeight="1">
       <c r="A25" s="9"/>
       <c r="B25" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="1:5" ht="20" customHeight="1">
+      <c r="E25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="20" customHeight="1">
       <c r="A26" s="9"/>
       <c r="B26" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C26" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="1:5" ht="20" customHeight="1">
+      <c r="E26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="20" customHeight="1">
       <c r="A27" s="9"/>
       <c r="B27" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="1:5" ht="20" customHeight="1">
+      <c r="E27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="20" customHeight="1">
       <c r="A28" s="7" t="s">
         <v>2</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C28" s="5"/>
       <c r="D28" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="1:5" ht="20" customHeight="1">
+        <v>23</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" ht="20" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>35</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="1:5" ht="20" customHeight="1">
+        <v>34</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="1:6" ht="20" customHeight="1">
       <c r="A30" s="9" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="1:5" ht="20" customHeight="1">
+        <v>24</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="20" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="1:5" ht="20" customHeight="1">
+        <v>24</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" ht="20" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" ht="20" customHeight="1">
+        <v>25</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" ht="20" customHeight="1">
       <c r="A33" s="9"/>
       <c r="B33" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="C33" s="5"/>
       <c r="D33" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" ht="20" customHeight="1">
+        <v>26</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" ht="20" customHeight="1">
       <c r="A34" s="9" t="s">
         <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>28</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C34" s="5"/>
       <c r="D34" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" ht="20" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" ht="20" customHeight="1">
       <c r="A35" s="9"/>
       <c r="B35" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>26</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C35" s="5"/>
       <c r="D35" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" ht="20" customHeight="1">
+        <v>25</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" ht="20" customHeight="1">
       <c r="A36" s="9"/>
       <c r="B36" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" ht="20" customHeight="1">
+      <c r="A37" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C36" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D36" s="5" t="s">
+      <c r="E37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" ht="20" customHeight="1">
+      <c r="A38" s="12"/>
+      <c r="B38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" ht="20" customHeight="1">
+      <c r="A39" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" s="5"/>
+    </row>
+    <row r="40" spans="1:6" ht="20" customHeight="1">
+      <c r="A40" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" ht="20" customHeight="1">
-      <c r="A37" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="E37" s="5"/>
-    </row>
-    <row r="38" spans="1:5" ht="20" customHeight="1">
-      <c r="A38" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" ht="20" customHeight="1">
-      <c r="A39" s="9"/>
-      <c r="B39" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E39" s="5"/>
-    </row>
-    <row r="40" spans="1:5" ht="20" customHeight="1">
-      <c r="A40" s="9"/>
-      <c r="B40" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" s="5"/>
-    </row>
-    <row r="41" spans="1:5" ht="20" customHeight="1">
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:6" ht="20" customHeight="1">
       <c r="A41" s="9"/>
       <c r="B41" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C41" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E41" s="5"/>
-    </row>
-    <row r="42" spans="1:5" ht="20" customHeight="1">
+      <c r="E41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="5"/>
+    </row>
+    <row r="42" spans="1:6" ht="20" customHeight="1">
       <c r="A42" s="9"/>
       <c r="B42" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="E42" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="20" customHeight="1">
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" ht="20" customHeight="1">
       <c r="A43" s="9"/>
       <c r="B43" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="20" customHeight="1">
-      <c r="A44" s="10"/>
-    </row>
-    <row r="45" spans="1:5" ht="20" customHeight="1">
-      <c r="A45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" ht="20" customHeight="1">
+        <v>76</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" ht="20" customHeight="1">
+      <c r="A44" s="9"/>
+      <c r="B44" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="1:6" ht="20" customHeight="1">
+      <c r="A45" s="9"/>
+      <c r="B45" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F45" s="5"/>
+    </row>
+    <row r="46" spans="1:6" ht="20" customHeight="1">
       <c r="A46" s="10"/>
     </row>
-    <row r="47" spans="1:5" ht="20" customHeight="1">
+    <row r="47" spans="1:6" ht="20" customHeight="1">
       <c r="A47" s="10"/>
     </row>
-    <row r="48" spans="1:5" ht="20" customHeight="1">
+    <row r="48" spans="1:6" ht="20" customHeight="1">
       <c r="A48" s="10"/>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
       <c r="A49" s="10"/>
     </row>
+    <row r="50" spans="1:1" ht="20" customHeight="1">
+      <c r="A50" s="10"/>
+    </row>
+    <row r="51" spans="1:1" ht="20" customHeight="1">
+      <c r="A51" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="A40:A45"/>
+    <mergeCell ref="A37:A38"/>
     <mergeCell ref="A11:A27"/>
     <mergeCell ref="A30:A33"/>
     <mergeCell ref="A34:A36"/>

</xml_diff>

<commit_message>
fix bug of list and view command for new script file format
</commit_message>
<xml_diff>
--- a/xdoc/test-case.xlsx
+++ b/xdoc/test-case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/dev/go/zentaoatf/xdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BABFEA7-606E-8C45-9D82-F7AC1981CAD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2DC53-EDEE-374F-B0F9-7873F64D8043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33280" windowHeight="20540" xr2:uid="{02BAE9CC-3948-864F-A7A3-2466404408E9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
   <si>
     <t>Up</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -163,10 +163,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>失败结果提交缺陷到禅道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CB</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -237,146 +233,157 @@
     <t xml:space="preserve">ztf.exe run . </t>
   </si>
   <si>
-    <t xml:space="preserve">ztf.exe scripts\all.cs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run scripts scripts\all.cs </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe scripts\all.cs scripts </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run logs\2019-09-04\result.txt </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe logs\2019-09-04\result.json </t>
+    <t xml:space="preserve">ztf.exe run scripts -s 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -t 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run scripts -t 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe list scripts\用例模块A scripts\tc-1.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe ls scripts\用例模块A\ scripts\tc-1.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 新闻  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe view scripts\用例模块A scripts\tc-1.php </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v scripts\用例模块A scripts\tc-1.php -k 1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v scripts\用例模块A\ scripts\tc-1.php -k 新闻  </t>
+  </si>
+  <si>
+    <t>ztf.exe win_line_break.bat</t>
+  </si>
+  <si>
+    <t>ztf.exe demo\sample</t>
+  </si>
+  <si>
+    <t>ztf demo\sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf demo\lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atf.exe sort demo\sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">atf.exe clean </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重排脚本中的步骤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除执行日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe -h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe co -m 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe co -p 1 -m 15 -l php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新用例到禅道(TODO)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe up -p 1 -l php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe demo\lang\php </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\2_webpage_extract.php</t>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\all.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe run demo\lang\php\all.cs scripts</t>
+  </si>
+  <si>
+    <t>ztf.exe run scripts demo\lang\php\all.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run log\006\result.txt </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t xml:space="preserve">ztf.exe -s 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run scripts -s 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -t 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run scripts -t 1 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe cr logs\2019-09-04 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe cb logs\2019-09-04 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe list scripts\用例模块A scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe ls scripts\用例模块A\ scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 新闻  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe view scripts\用例模块A scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v scripts\用例模块A scripts\tc-1.php -k 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v scripts\用例模块A\ scripts\tc-1.php -k 新闻  </t>
-  </si>
-  <si>
-    <t>ztf.exe win_line_break.bat</t>
-  </si>
-  <si>
-    <t>ztf.exe demo\sample</t>
-  </si>
-  <si>
-    <t>ztf demo\sample</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf demo\lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>atf.exe sort demo\sample</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">atf.exe clean </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重排脚本中的步骤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>清除执行日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe -h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe set</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe co -m 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe co -p 1 -m 15 -l php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更新用例到禅道(TODO)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe up -p 1 -l php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Priority</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe demo\lang\php </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang\php\</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang\php\2_webpage_extract.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe cr log\003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe cb logs\003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将失败结果提交缺陷到禅道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail GoCui中文乱码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -434,8 +441,15 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +459,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14996795556505021"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,7 +561,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -581,19 +601,40 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -910,20 +951,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6013D07F-3FC9-2B42-A079-965085852FDE}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="58.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="72.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="39.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="6" max="6" width="32.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20" customHeight="1">
@@ -934,70 +976,70 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1">
-      <c r="A2" s="9" t="s">
+    <row r="2" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A2" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="9"/>
-      <c r="B3" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16" t="s">
+      <c r="E2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1">
+      <c r="A3" s="13"/>
+      <c r="B3" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1">
-      <c r="A4" s="9"/>
-      <c r="B4" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="E3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A4" s="13"/>
+      <c r="B4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="14">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>85</v>
+      <c r="E4" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
@@ -1005,7 +1047,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1014,32 +1056,32 @@
         <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="5" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1048,50 +1090,50 @@
         <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="15" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="24" customFormat="1" ht="20" customHeight="1">
+      <c r="A8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="14"/>
+      <c r="B8" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="23"/>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">
       <c r="A9" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1100,444 +1142,472 @@
         <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A11" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="14">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A16" s="13"/>
+      <c r="B16" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="14">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A18" s="13"/>
+      <c r="B18" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A19" s="13"/>
+      <c r="B19" s="14" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1">
-      <c r="A11" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1">
-      <c r="A12" s="9"/>
-      <c r="B12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1">
-      <c r="A13" s="9"/>
-      <c r="B13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1">
-      <c r="A14" s="9"/>
-      <c r="B14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="5">
-        <v>1</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1">
-      <c r="A15" s="9"/>
-      <c r="B15" s="5" t="s">
+      <c r="C19" s="14"/>
+      <c r="D19" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A20" s="13"/>
+      <c r="B20" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A22" s="13"/>
+      <c r="B22" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22" s="14"/>
+      <c r="D22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A23" s="13"/>
+      <c r="B23" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A24" s="13"/>
+      <c r="B24" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1">
-      <c r="A16" s="9"/>
-      <c r="B16" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" ht="20" customHeight="1">
-      <c r="A17" s="9"/>
-      <c r="B17" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="C17" s="5">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" ht="20" customHeight="1">
-      <c r="A18" s="9"/>
-      <c r="B18" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" ht="20" customHeight="1">
-      <c r="A19" s="9"/>
-      <c r="B19" s="5" t="s">
+      <c r="C24" s="14"/>
+      <c r="D24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A25" s="13"/>
+      <c r="B25" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="6"/>
-    </row>
-    <row r="20" spans="1:6" ht="20" customHeight="1">
-      <c r="A20" s="9"/>
-      <c r="B20" s="5" t="s">
+      <c r="C25" s="14"/>
+      <c r="D25" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" ht="20" customHeight="1">
-      <c r="A21" s="9"/>
-      <c r="B21" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" ht="20" customHeight="1">
-      <c r="A22" s="9"/>
-      <c r="B22" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="20" customHeight="1">
-      <c r="A23" s="9"/>
-      <c r="B23" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" ht="20" customHeight="1">
-      <c r="A24" s="9"/>
-      <c r="B24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" ht="20" customHeight="1">
-      <c r="A25" s="9"/>
-      <c r="B25" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" ht="20" customHeight="1">
-      <c r="A26" s="9"/>
-      <c r="B26" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="6"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="20" customHeight="1">
-      <c r="A27" s="9"/>
+      <c r="A27" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="B27" s="5" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" ht="20" customHeight="1">
-      <c r="A28" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="21" customFormat="1" ht="20" customHeight="1">
+      <c r="A28" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="20" customHeight="1">
-      <c r="A29" s="7" t="s">
-        <v>35</v>
+      <c r="A29" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F29" s="6"/>
     </row>
     <row r="30" spans="1:6" ht="20" customHeight="1">
-      <c r="A30" s="9" t="s">
-        <v>5</v>
-      </c>
+      <c r="A30" s="9"/>
       <c r="B30" s="5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F30" s="6"/>
     </row>
     <row r="31" spans="1:6" ht="20" customHeight="1">
       <c r="A31" s="9"/>
       <c r="B31" s="5" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F31" s="6"/>
     </row>
     <row r="32" spans="1:6" ht="20" customHeight="1">
       <c r="A32" s="9"/>
       <c r="B32" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A33" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F33" s="15"/>
+    </row>
+    <row r="34" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A34" s="13"/>
+      <c r="B34" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" ht="20" customHeight="1">
-      <c r="A33" s="9"/>
-      <c r="B33" s="5" t="s">
+      <c r="E34" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F34" s="15"/>
+    </row>
+    <row r="35" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A35" s="13"/>
+      <c r="B35" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F35" s="15"/>
+    </row>
+    <row r="36" spans="1:6" ht="20" customHeight="1">
+      <c r="A36" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="20" customHeight="1">
-      <c r="A34" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" ht="20" customHeight="1">
-      <c r="A35" s="9"/>
-      <c r="B35" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" ht="20" customHeight="1">
-      <c r="A36" s="9"/>
-      <c r="B36" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F36" s="6"/>
     </row>
     <row r="37" spans="1:6" ht="20" customHeight="1">
-      <c r="A37" s="11" t="s">
-        <v>80</v>
-      </c>
+      <c r="A37" s="12"/>
       <c r="B37" s="5" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" ht="20" customHeight="1">
-      <c r="A38" s="12"/>
-      <c r="B38" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F38" s="6"/>
+    <row r="38" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+      <c r="A38" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="14"/>
     </row>
     <row r="39" spans="1:6" ht="20" customHeight="1">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="9" t="s">
         <v>37</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="E39" s="5" t="s">
         <v>44</v>
@@ -1545,31 +1615,29 @@
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" ht="20" customHeight="1">
-      <c r="A40" s="9" t="s">
-        <v>38</v>
-      </c>
+      <c r="A40" s="9"/>
       <c r="B40" s="5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="1:6" ht="20" customHeight="1">
       <c r="A41" s="9"/>
       <c r="B41" s="5" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E41" s="5" t="s">
+      <c r="D41" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F41" s="5"/>
@@ -1577,58 +1645,47 @@
     <row r="42" spans="1:6" ht="20" customHeight="1">
       <c r="A42" s="9"/>
       <c r="B42" s="5" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>43</v>
+      <c r="D42" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" ht="20" customHeight="1">
       <c r="A43" s="9"/>
       <c r="B43" s="5" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" ht="20" customHeight="1">
       <c r="A44" s="9"/>
       <c r="B44" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>42</v>
       </c>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" ht="20" customHeight="1">
-      <c r="A45" s="9"/>
-      <c r="B45" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="F45" s="5"/>
+      <c r="A45" s="10"/>
     </row>
     <row r="46" spans="1:6" ht="20" customHeight="1">
       <c r="A46" s="10"/>
@@ -1644,20 +1701,17 @@
     </row>
     <row r="50" spans="1:1" ht="20" customHeight="1">
       <c r="A50" s="10"/>
-    </row>
-    <row r="51" spans="1:1" ht="20" customHeight="1">
-      <c r="A51" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A40:A45"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A11:A27"/>
-    <mergeCell ref="A30:A33"/>
-    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A11:A26"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A35"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix a bug when group has [steps] but no [expects]
</commit_message>
<xml_diff>
--- a/xdoc/test-case.xlsx
+++ b/xdoc/test-case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/dev/go/zentaoatf/xdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C2DC53-EDEE-374F-B0F9-7873F64D8043}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D07A9B-2F37-4D4B-95E5-060B8A6AD381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33280" windowHeight="20540" xr2:uid="{02BAE9CC-3948-864F-A7A3-2466404408E9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="92">
   <si>
     <t>Up</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -167,14 +167,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>测试windows换行符兼容性</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Compatibility</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Demo Script</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -242,30 +234,6 @@
     <t xml:space="preserve">ztf.exe run scripts -t 1 </t>
   </si>
   <si>
-    <t xml:space="preserve">ztf.exe list scripts\用例模块A scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe ls scripts\用例模块A\ scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -l scripts\用例模块A scripts\tc-1.php -k 新闻  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe view scripts\用例模块A scripts\tc-1.php </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v scripts\用例模块A scripts\tc-1.php -k 1  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v scripts\用例模块A\ scripts\tc-1.php -k 新闻  </t>
-  </si>
-  <si>
-    <t>ztf.exe win_line_break.bat</t>
-  </si>
-  <si>
     <t>ztf.exe demo\sample</t>
   </si>
   <si>
@@ -281,14 +249,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>atf.exe sort demo\sample</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">atf.exe clean </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Other</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -376,6 +336,46 @@
   </si>
   <si>
     <t>fail GoCui中文乱码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe list demo\lang\php demo\sample\8_skip.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe ls demo\lang\php demo\sample\8_skip.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe -l demo\lang\php demo\sample\8_skip.php -k -1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -l demo\lang\php demo\sample\8_skip.php -k matches </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe view demo\lang\php demo\sample\8_skip.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v demo\lang\php demo\sample\8_skip.php -k -1  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v demo\lang\php demo\sample\8_skip.php -k matches </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail 不带[group]的有问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe sort demo\sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe clean </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -561,7 +561,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -586,9 +586,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -601,6 +598,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,6 +638,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -951,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6013D07F-3FC9-2B42-A079-965085852FDE}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1"/>
@@ -976,78 +982,78 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="14">
+      <c r="B2" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="19" customFormat="1" ht="20" customHeight="1">
+      <c r="A3" s="14"/>
+      <c r="B3" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A4" s="14"/>
+      <c r="B4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="20" customHeight="1">
+      <c r="A5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="18" customFormat="1" ht="20" customHeight="1">
-      <c r="A3" s="13"/>
-      <c r="B3" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A4" s="13"/>
-      <c r="B4" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="14">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1">
-      <c r="A5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -1056,32 +1062,32 @@
         <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1">
-      <c r="A6" s="9"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
         <v>30</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="5" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1090,50 +1096,50 @@
         <v>14</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="24" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="25" customFormat="1" ht="20" customHeight="1">
+      <c r="A8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="23"/>
+      <c r="B8" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F8" s="24"/>
     </row>
     <row r="9" spans="1:6" ht="20" customHeight="1">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">
-      <c r="A10" s="9"/>
+      <c r="A10" s="8"/>
       <c r="B10" s="5" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1142,276 +1148,276 @@
         <v>14</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A11" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="15">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A12" s="14"/>
+      <c r="B12" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A13" s="14"/>
+      <c r="B13" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A14" s="14"/>
+      <c r="B14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="15">
+        <v>1</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A15" s="14"/>
+      <c r="B15" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A16" s="14"/>
+      <c r="B16" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A18" s="14"/>
+      <c r="B18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A19" s="14"/>
+      <c r="B19" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A20" s="14"/>
+      <c r="B20" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A21" s="14"/>
+      <c r="B21" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A22" s="14"/>
+      <c r="B22" s="15" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A11" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="14">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="14">
-        <v>1</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14" t="s">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A23" s="14"/>
+      <c r="B23" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A24" s="14"/>
+      <c r="B24" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="14">
-        <v>1</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A15" s="13"/>
-      <c r="B15" s="14" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A25" s="14"/>
+      <c r="B25" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A16" s="13"/>
-      <c r="B16" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C17" s="14">
-        <v>1</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A22" s="13"/>
-      <c r="B22" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A24" s="13"/>
-      <c r="B24" s="14" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A26" s="14"/>
+      <c r="B26" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A25" s="13"/>
-      <c r="B25" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>76</v>
+      <c r="E26" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="20" customHeight="1">
@@ -1419,295 +1425,297 @@
         <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="21" customFormat="1" ht="20" customHeight="1">
-      <c r="A28" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="22" customFormat="1" ht="20" customHeight="1">
+      <c r="A28" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E28" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F28" s="20" t="s">
-        <v>93</v>
+      <c r="B28" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="20" customHeight="1">
-      <c r="A29" s="9" t="s">
+      <c r="A29" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F29" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="20" customHeight="1">
-      <c r="A30" s="9"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="5" t="s">
-        <v>58</v>
+        <v>83</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
         <v>24</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F30" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="20" customHeight="1">
-      <c r="A31" s="9"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="5" t="s">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F31" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="20" customHeight="1">
-      <c r="A32" s="9"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="5" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
         <v>26</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A33" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A33" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14" t="s">
+      <c r="B33" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E33" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F33" s="15"/>
-    </row>
-    <row r="34" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A34" s="13"/>
-      <c r="B34" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14" t="s">
+      <c r="E33" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F33" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A34" s="14"/>
+      <c r="B34" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E34" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F34" s="15"/>
-    </row>
-    <row r="35" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
-      <c r="A35" s="13"/>
-      <c r="B35" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14" t="s">
+      <c r="E34" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F34" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A35" s="14"/>
+      <c r="B35" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F35" s="15"/>
-    </row>
-    <row r="36" spans="1:6" ht="20" customHeight="1">
-      <c r="A36" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F36" s="6"/>
+      <c r="E35" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35" s="16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="13" customFormat="1" ht="20" customHeight="1">
+      <c r="A36" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="37" spans="1:6" ht="20" customHeight="1">
-      <c r="A37" s="12"/>
+      <c r="A37" s="11"/>
       <c r="B37" s="5" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" s="16" customFormat="1" ht="20" customHeight="1">
+        <v>41</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A38" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F38" s="15"/>
+    </row>
+    <row r="39" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A39" s="14"/>
+      <c r="B39" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="15"/>
+    </row>
+    <row r="40" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A40" s="14"/>
+      <c r="B40" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="15"/>
+    </row>
+    <row r="41" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A41" s="14"/>
+      <c r="B41" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6" ht="20" customHeight="1">
-      <c r="A39" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5" t="s">
+      <c r="E41" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F41" s="15"/>
+    </row>
+    <row r="42" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A42" s="14"/>
+      <c r="B42" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F39" s="5"/>
-    </row>
-    <row r="40" spans="1:6" ht="20" customHeight="1">
-      <c r="A40" s="9"/>
-      <c r="B40" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" s="5"/>
-    </row>
-    <row r="41" spans="1:6" ht="20" customHeight="1">
-      <c r="A41" s="9"/>
-      <c r="B41" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F41" s="5"/>
-    </row>
-    <row r="42" spans="1:6" ht="20" customHeight="1">
-      <c r="A42" s="9"/>
-      <c r="B42" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F42" s="5"/>
-    </row>
-    <row r="43" spans="1:6" ht="20" customHeight="1">
-      <c r="A43" s="9"/>
-      <c r="B43" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F43" s="5"/>
+      <c r="F42" s="15"/>
+    </row>
+    <row r="43" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="A43" s="14"/>
+      <c r="B43" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="15"/>
     </row>
     <row r="44" spans="1:6" ht="20" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" ht="20" customHeight="1">
-      <c r="A45" s="10"/>
+      <c r="A45" s="9"/>
     </row>
     <row r="46" spans="1:6" ht="20" customHeight="1">
-      <c r="A46" s="10"/>
+      <c r="A46" s="9"/>
     </row>
     <row r="47" spans="1:6" ht="20" customHeight="1">
-      <c r="A47" s="10"/>
+      <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:6" ht="20" customHeight="1">
-      <c r="A48" s="10"/>
+      <c r="A48" s="9"/>
     </row>
     <row r="49" spans="1:1" ht="20" customHeight="1">
-      <c r="A49" s="10"/>
-    </row>
-    <row r="50" spans="1:1" ht="20" customHeight="1">
-      <c r="A50" s="10"/>
+      <c r="A49" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A39:A44"/>
+    <mergeCell ref="A38:A43"/>
     <mergeCell ref="A36:A37"/>
     <mergeCell ref="A11:A26"/>
     <mergeCell ref="A29:A32"/>

</xml_diff>

<commit_message>
fix a enabledelayedexpansion related bug for bat script
</commit_message>
<xml_diff>
--- a/xdoc/test-case.xlsx
+++ b/xdoc/test-case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/dev/go/zentaoatf/xdoc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D07A9B-2F37-4D4B-95E5-060B8A6AD381}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20098C7F-4784-C64D-BEFA-43F784B3B67A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33280" windowHeight="20540" xr2:uid="{02BAE9CC-3948-864F-A7A3-2466404408E9}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="93">
   <si>
     <t>Up</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -234,148 +234,153 @@
     <t xml:space="preserve">ztf.exe run scripts -t 1 </t>
   </si>
   <si>
+    <t>ztf demo\sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf demo\lang</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重排脚本中的步骤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除执行日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe -h</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe set</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pass</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe co -m 15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe co -p 1 -m 15 -l php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新用例到禅道(TODO)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe up -p 1 -l php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Priority</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe demo\lang\php </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\2_webpage_extract.php</t>
+  </si>
+  <si>
+    <t>ztf.exe demo\lang\php\all.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe run demo\lang\php\all.cs scripts</t>
+  </si>
+  <si>
+    <t>ztf.exe run scripts demo\lang\php\all.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe run log\006\result.txt </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -s 1 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe cr log\003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe cb logs\003</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>将失败结果提交缺陷到禅道</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail GoCui中文乱码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe list demo\lang\php demo\sample\8_skip.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe ls demo\lang\php demo\sample\8_skip.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe -l demo\lang\php demo\sample\8_skip.php -k -1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -l demo\lang\php demo\sample\8_skip.php -k matches </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe view demo\lang\php demo\sample\8_skip.php</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v demo\lang\php demo\sample\8_skip.php -k -1  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe -v demo\lang\php demo\sample\8_skip.php -k matches </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail 不带[group]的有问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ztf.exe sort demo\sample</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ztf.exe clean </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>ztf.exe demo\sample</t>
-  </si>
-  <si>
-    <t>ztf demo\sample</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf demo\lang</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Other</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重排脚本中的步骤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>清除执行日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe -h</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe set</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>pass</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe co -m 15</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe co -p 1 -m 15 -l php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>更新用例到禅道(TODO)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe up -p 1 -l php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Priority</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe demo\lang\php </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang\php\</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang\php\2_webpage_extract.php</t>
-  </si>
-  <si>
-    <t>ztf.exe demo\lang\php\all.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe run demo\lang\php\all.cs scripts</t>
-  </si>
-  <si>
-    <t>ztf.exe run scripts demo\lang\php\all.cs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe run log\006\result.txt </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -s 1 </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe cr log\003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe cb logs\003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>将失败结果提交缺陷到禅道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fail GoCui中文乱码</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe list demo\lang\php demo\sample\8_skip.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe ls demo\lang\php demo\sample\8_skip.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe -l demo\lang\php demo\sample\8_skip.php -k -1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -l demo\lang\php demo\sample\8_skip.php -k matches </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe view demo\lang\php demo\sample\8_skip.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v demo\lang\php demo\sample\8_skip.php -k -1  </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe -v demo\lang\php demo\sample\8_skip.php -k matches </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fail 不带[group]的有问题</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ztf.exe sort demo\sample</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ztf.exe clean </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail bat 2,3脚本报错</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -960,7 +965,7 @@
   <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" customHeight="1"/>
@@ -982,7 +987,7 @@
         <v>8</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>10</v>
@@ -1011,13 +1016,13 @@
         <v>42</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="19" customFormat="1" ht="20" customHeight="1">
       <c r="A3" s="14"/>
       <c r="B3" s="18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18" t="s">
@@ -1027,13 +1032,13 @@
         <v>42</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A4" s="14"/>
       <c r="B4" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="15">
         <v>1</v>
@@ -1045,7 +1050,7 @@
         <v>41</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="20" customHeight="1">
@@ -1065,13 +1070,13 @@
         <v>41</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="20" customHeight="1">
       <c r="A6" s="8"/>
       <c r="B6" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
@@ -1081,13 +1086,13 @@
         <v>41</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="20" customHeight="1">
       <c r="A7" s="8"/>
       <c r="B7" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -1099,7 +1104,7 @@
         <v>41</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="25" customFormat="1" ht="20" customHeight="1">
@@ -1111,7 +1116,7 @@
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>41</v>
@@ -1133,13 +1138,13 @@
         <v>41</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20" customHeight="1">
       <c r="A10" s="8"/>
       <c r="B10" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" s="5">
         <v>1</v>
@@ -1151,7 +1156,7 @@
         <v>41</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1171,7 +1176,7 @@
         <v>41</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1189,7 +1194,7 @@
         <v>41</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1205,7 +1210,7 @@
         <v>41</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1223,7 +1228,7 @@
         <v>41</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1239,13 +1244,13 @@
         <v>41</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A16" s="14"/>
       <c r="B16" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
@@ -1255,13 +1260,13 @@
         <v>41</v>
       </c>
       <c r="F16" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A17" s="14"/>
       <c r="B17" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C17" s="15">
         <v>1</v>
@@ -1273,13 +1278,13 @@
         <v>41</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A18" s="14"/>
       <c r="B18" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
@@ -1289,13 +1294,13 @@
         <v>41</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A19" s="14"/>
       <c r="B19" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
@@ -1305,13 +1310,13 @@
         <v>41</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A20" s="14"/>
       <c r="B20" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
@@ -1321,13 +1326,13 @@
         <v>41</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A21" s="14"/>
       <c r="B21" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
@@ -1337,13 +1342,13 @@
         <v>41</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A22" s="14"/>
       <c r="B22" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
@@ -1353,13 +1358,13 @@
         <v>41</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A23" s="14"/>
       <c r="B23" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
@@ -1369,7 +1374,7 @@
         <v>41</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1385,7 +1390,7 @@
         <v>41</v>
       </c>
       <c r="F24" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1401,7 +1406,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1417,7 +1422,7 @@
         <v>41</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="20" customHeight="1">
@@ -1425,7 +1430,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
@@ -1435,7 +1440,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="22" customFormat="1" ht="20" customHeight="1">
@@ -1443,17 +1448,17 @@
         <v>34</v>
       </c>
       <c r="B28" s="21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="21"/>
       <c r="D28" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F28" s="21" t="s">
         <v>80</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F28" s="21" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="20" customHeight="1">
@@ -1461,7 +1466,7 @@
         <v>5</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5" t="s">
@@ -1471,13 +1476,13 @@
         <v>41</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="20" customHeight="1">
       <c r="A30" s="8"/>
       <c r="B30" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
@@ -1487,13 +1492,13 @@
         <v>41</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="20" customHeight="1">
       <c r="A31" s="8"/>
       <c r="B31" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5" t="s">
@@ -1503,13 +1508,13 @@
         <v>41</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="20" customHeight="1">
       <c r="A32" s="8"/>
       <c r="B32" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5" t="s">
@@ -1519,7 +1524,7 @@
         <v>41</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1527,7 +1532,7 @@
         <v>6</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15" t="s">
@@ -1537,13 +1542,13 @@
         <v>41</v>
       </c>
       <c r="F33" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A34" s="14"/>
       <c r="B34" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
@@ -1553,13 +1558,13 @@
         <v>41</v>
       </c>
       <c r="F34" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A35" s="14"/>
       <c r="B35" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
@@ -1569,41 +1574,41 @@
         <v>41</v>
       </c>
       <c r="F35" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="13" customFormat="1" ht="20" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C36" s="12"/>
       <c r="D36" s="12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>41</v>
       </c>
       <c r="F36" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="20" customHeight="1">
       <c r="A37" s="11"/>
       <c r="B37" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E37" s="5" t="s">
         <v>41</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
@@ -1611,7 +1616,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>55</v>
+        <v>91</v>
       </c>
       <c r="C38" s="15"/>
       <c r="D38" s="15" t="s">
@@ -1620,12 +1625,14 @@
       <c r="E38" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="F38" s="15"/>
+      <c r="F38" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="39" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A39" s="14"/>
       <c r="B39" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C39" s="15"/>
       <c r="D39" s="15" t="s">
@@ -1634,12 +1641,14 @@
       <c r="E39" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="15"/>
+      <c r="F39" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="40" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A40" s="14"/>
       <c r="B40" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C40" s="15"/>
       <c r="D40" s="26" t="s">
@@ -1648,26 +1657,30 @@
       <c r="E40" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="15"/>
-    </row>
-    <row r="41" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
+      <c r="F40" s="16" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="22" customFormat="1" ht="20" customHeight="1">
       <c r="A41" s="14"/>
-      <c r="B41" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15" t="s">
+      <c r="B41" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="F41" s="15"/>
+      <c r="F41" s="21" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="42" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A42" s="14"/>
       <c r="B42" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="15" t="s">
@@ -1676,12 +1689,14 @@
       <c r="E42" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F42" s="15"/>
+      <c r="F42" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="43" spans="1:6" s="17" customFormat="1" ht="20" customHeight="1">
       <c r="A43" s="14"/>
       <c r="B43" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="15"/>
       <c r="D43" s="15" t="s">
@@ -1690,7 +1705,9 @@
       <c r="E43" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="F43" s="15"/>
+      <c r="F43" s="16" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="44" spans="1:6" ht="20" customHeight="1">
       <c r="A44" s="9"/>

</xml_diff>